<commit_message>
Premium Calculator works, summary message gives back the right atris
</commit_message>
<xml_diff>
--- a/Zsuzsi_Schliffer/Training/Training1/DriverAgeExcel.xlsx
+++ b/Zsuzsi_Schliffer/Training/Training1/DriverAgeExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsuzsa\Documents\git_sandbox\Zsuzsi_Schliffer\Training\Training1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B067B7F-37A2-49F1-843D-ACD5474C772E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07B751E-3BEC-42D4-BDC5-36CB02491122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="915"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skye Lookup Input" sheetId="41" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,12 +215,14 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Montserrat"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color theme="1" tint="0.14999847407452621"/>
+      <color theme="1" tint="0.14996795556505021"/>
       <name val="Montserrat"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="5">
@@ -244,7 +246,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,8 +276,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -293,7 +295,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -628,14 +630,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:IV5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -948,10 +950,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -960,12 +962,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -1023,7 +1025,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">Algorithm!B4</f>
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1032,17 +1034,17 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">Algorithm!B5</f>
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
@@ -1072,11 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,8 +1110,8 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <f ca="1">INT(YEARFRAC(TODAY(),B1))</f>
-        <v>119</v>
+        <f ca="1">IF('Skye Lookup Input'!D2=0,0,INT(YEARFRAC(TODAY(),B1)))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,18 +1119,18 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <f ca="1">INT(YEARFRAC(TODAY(),B2))</f>
-        <v>119</v>
+        <f ca="1">IF('Skye Lookup Input'!D3=0,0,INT(YEARFRAC(TODAY(),B1)))</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
minor changes: Home button redirects to Zone, after selecting the zip Code the City appears, mandatory atris enabled, different type of error messages, summary message format changes
</commit_message>
<xml_diff>
--- a/Zsuzsi_Schliffer/Training/Training1/DriverAgeExcel.xlsx
+++ b/Zsuzsi_Schliffer/Training/Training1/DriverAgeExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsuzsa\Documents\git_sandbox\Zsuzsi_Schliffer\Training\Training1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07B751E-3BEC-42D4-BDC5-36CB02491122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D4382-94A0-47A3-8924-2DCEBD0B9890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skye Lookup Input" sheetId="41" r:id="rId1"/>
@@ -637,7 +637,7 @@
   <dimension ref="A1:IV5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1119,7 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <f ca="1">IF('Skye Lookup Input'!D3=0,0,INT(YEARFRAC(TODAY(),B1)))</f>
+        <f ca="1">IF('Skye Lookup Input'!D3=0,0,INT(YEARFRAC(TODAY(),B2)))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>